<commit_message>
preparing temp data for occ mod
</commit_message>
<xml_diff>
--- a/TemperatureData/Audobon/0201.xlsx
+++ b/TemperatureData/Audobon/0201.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvmoffice.sharepoint.com/sites/TeamMosher/Shared Documents/General/People/Scott, Reed/FieldWork2022/HoboLoggerData/Audobon/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitrepos\VTADS\TemperatureData\Audobon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{112675F0-24D5-4EA3-8DF8-E93D7E7283C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B06FB5-5D12-45A5-A18E-8FB1BE144B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0201" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Plot Title: 21422132</t>
   </si>
@@ -50,9 +50,6 @@
     <t>End Of File (LGR S/N: 21422132)</t>
   </si>
   <si>
-    <t>Logged</t>
-  </si>
-  <si>
     <t>#Hobo Logger data for Audobon Center</t>
   </si>
   <si>
@@ -66,6 +63,9 @@
   </si>
   <si>
     <t>#logger was collected on 08/17/2022 at 2:47</t>
+  </si>
+  <si>
+    <t>#All data after this date / time was deleted</t>
   </si>
 </sst>
 </file>
@@ -907,9 +907,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6075"/>
+  <dimension ref="A1:H6062"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A6034" workbookViewId="0">
+      <selection activeCell="A6075" sqref="A6063:XFD6075"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -85787,188 +85789,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6063" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6063">
-        <v>6061</v>
-      </c>
-      <c r="B6063" s="1">
-        <v>44790.625</v>
-      </c>
-      <c r="C6063">
-        <v>77.573999999999998</v>
-      </c>
-      <c r="D6063">
-        <v>5632</v>
-      </c>
-    </row>
-    <row r="6064" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6064">
-        <v>6062</v>
-      </c>
-      <c r="B6064" s="1">
-        <v>44790.635416666664</v>
-      </c>
-      <c r="C6064">
-        <v>81.266000000000005</v>
-      </c>
-      <c r="D6064">
-        <v>2816</v>
-      </c>
-    </row>
-    <row r="6065" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6065">
-        <v>6063</v>
-      </c>
-      <c r="B6065" s="1">
-        <v>44790.645833333336</v>
-      </c>
-      <c r="C6065">
-        <v>78.623999999999995</v>
-      </c>
-      <c r="D6065">
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="6066" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6066">
-        <v>6064</v>
-      </c>
-      <c r="B6066" s="1">
-        <v>44790.65625</v>
-      </c>
-      <c r="C6066">
-        <v>77.748999999999995</v>
-      </c>
-      <c r="D6066">
-        <v>2304</v>
-      </c>
-    </row>
-    <row r="6067" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6067">
-        <v>6065</v>
-      </c>
-      <c r="B6067" s="1">
-        <v>44790.666666666664</v>
-      </c>
-      <c r="C6067">
-        <v>77.224999999999994</v>
-      </c>
-      <c r="D6067">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="6068" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6068">
-        <v>6066</v>
-      </c>
-      <c r="B6068" s="1">
-        <v>44790.677083333336</v>
-      </c>
-      <c r="C6068">
-        <v>75.659000000000006</v>
-      </c>
-      <c r="D6068">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="6069" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6069">
-        <v>6067</v>
-      </c>
-      <c r="B6069" s="1">
-        <v>44790.6875</v>
-      </c>
-      <c r="C6069">
-        <v>79.677999999999997</v>
-      </c>
-      <c r="D6069">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6070" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6070">
-        <v>6068</v>
-      </c>
-      <c r="B6070" s="1">
-        <v>44790.697916666664</v>
-      </c>
-      <c r="C6070">
-        <v>77.573999999999998</v>
-      </c>
-      <c r="D6070">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6071" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6071">
-        <v>6069</v>
-      </c>
-      <c r="B6071" s="1">
-        <v>44790.708333333336</v>
-      </c>
-      <c r="C6071">
-        <v>74.963999999999999</v>
-      </c>
-      <c r="D6071">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6072" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6072">
-        <v>6070</v>
-      </c>
-      <c r="B6072" s="1">
-        <v>44790.71875</v>
-      </c>
-      <c r="C6072">
-        <v>73.233999999999995</v>
-      </c>
-      <c r="D6072">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6073" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6073">
-        <v>6071</v>
-      </c>
-      <c r="B6073" s="1">
-        <v>44790.729166666664</v>
-      </c>
-      <c r="C6073">
-        <v>73.926000000000002</v>
-      </c>
-      <c r="D6073">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6074" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6074">
-        <v>6072</v>
-      </c>
-      <c r="B6074" s="1">
-        <v>44790.736435185187</v>
-      </c>
-      <c r="E6074" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6074" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6075" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6075">
-        <v>6073</v>
-      </c>
-      <c r="B6075" s="1">
-        <v>44790.736562500002</v>
-      </c>
-      <c r="G6075" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6075" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -85976,36 +85796,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -86026,15 +85851,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D153441376FC57458463DD41A74D2A65" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="99899fcf8d148fc44648e386da3fce05">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f61aad6-7023-4354-b4be-ac6efb5d4555" xmlns:ns3="94106a43-364c-4431-a764-9e3dd608a139" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6bf73413ded88cc8211ff1c3e53e5b06" ns2:_="" ns3:_="">
     <xsd:import namespace="6f61aad6-7023-4354-b4be-ac6efb5d4555"/>
@@ -86261,6 +86077,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40110A68-6162-4279-A197-0AF5434424FE}">
   <ds:schemaRefs>
@@ -86273,14 +86098,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AD70997-9A33-41B6-84F3-0D801C69D19E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02D6A30A-D963-4164-8A41-3CA1C9F39EED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -86297,4 +86114,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AD70997-9A33-41B6-84F3-0D801C69D19E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>